<commit_message>
added english word library for alias and literal lookups in where predicates
</commit_message>
<xml_diff>
--- a/generated_queries.xlsx
+++ b/generated_queries.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PRESENT city . Population and CountryCode IN ( FROM city table WHAT ARE city . country_id , city . ID AND THEN HAVING COUNT ( ID ) less than 19 ORDER BY country_id ASC ) as sq_alias AND THEN GROUP AUTOMATIC</t>
+          <t>join course with department on course . deptId equals department . id AND THEN FROM course table WHAT ARE THE count ( title ) , department . deptId AND THEN WHAT IS count ( id ) , course . departmentName , id and _CN_ FROM department AND THEN LIMIT 44 GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -454,7 +454,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FROM the city table WHAT IS THE count ( Population ) , Name and District where last_update is equal to bar AND THEN ORDER BY Name DESC GROUP AUTOMATICALLY LIMIT 47</t>
+          <t>IN Salaries as Ss where Salary is equal to 354 and Salary is greater than 510 WHAT IS THE Salaries . FromDate and EmployeeNumber</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FROM table course PRESENT id and course . title and code where title equals foo or id equals bar AND THEN LIMIT 37</t>
+          <t>IN the staff table WHAT ARE staff . username and count ( password ) and picture GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>natural join customer with store AND THEN FROM customer as cr SELECT customer_id and active AND THEN WHAT ARE THE address_id and customer . manager_staff_id FROM the store table as se AND THEN ORDER BY manager_staff_id DESC HAVING AVG ( address_id ) less than 114</t>
+          <t>FIND count ( endTime ) , the count of ( termId ) FROM ( FIND term . year and count ( endDate ) , term . endDate IN the term table where termPeriod IN ( DISPLAY id FROM TABLE term ) and endDate equals bar GROUP AUTOMATIC ) as sq_alias GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>natural join staff with store AND THEN IN the staff table as sf RETRIEVE password and staff . active and last_update and count ( staff_id ) AND THEN SELECT the count of ( store_id ) and count ( address_id ) , count ( store_id ) and count ( last_update ) and manager_staff_id , the count of ( address_id ) FROM store table where last_update equals foo AND THEN GROUP BY AUTOMATIC</t>
+          <t>WHAT IS THE DepartmentManager . EmployeeNumber , count ( EmployeeNumber ) FROM table DepartmentManager as Dr where EmployeeNumber is equal to foo and EmployeeNumber equals bar GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>natural join Titles with Employees AND THEN FROM table Titles where ToDate is equal to bar and Title is equal to bar FIND Title , FromDate and Employees . EmployeeNumber , count ( EmployeeNumber ) AND THEN WHAT ARE THE FirstName and the count of ( FirstName ) where EmployeeNumber is equal to bar IN Employees table AND THEN GROUP AUTOMATIC</t>
+          <t>natural join city with countrylanguage AND THEN SHOW ME District and the count of ( city_id ) IN city AND THEN SELECT city . IsOfficial , count ( Language ) and countrylanguage . CountryCode FROM table countrylanguage AND THEN HAVING COUNT ( CountryCode ) greater than 112 GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>natural join Titles with Employees AND THEN IN Titles as Ts FIND EmployeeNumber , ToDate where FromDate is equal to bar and Title IN ( SELECT Title IN TABLE Employees ) AND THEN FROM Employees table FIND Employees . EmployeeNumber , HireDate , Titles . Gender AND THEN GROUP BY AUTOMATIC</t>
+          <t>natural join city with countrylanguage AND THEN IN city as cy WHAT IS THE city . District and ID , the sum of ( Population ) , last_update where last_update equals bar or CountryCode equals bar AND THEN SHOW ME the sum of ( Percentage ) , count ( CountryCode ) and countrylanguage . CountryCode where Language equals bar IN countrylanguage table AND THEN HAVING AVG ( CountryCode ) greater than 191 GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SHOW ME city . Name , the average of ( Population ) , District IN the city table as cy where Name equals foo and Name equals bar AND THEN IN the country table as cy WHAT IS THE SurfaceArea and average ( SurfaceArea ) , country . last_update and Capital AND THEN natural join city with country AND THEN LIMIT 46 GROUP AUTOMATIC HAVING AVG ( last_update ) equal to 151</t>
+          <t>IN DepartmentManager as Dr where EmployeeNumber equals bar and FromDate IN ( SELECT DepartmentNumber FROM TABLE DepartmentManager ) PRESENT the count of ( ToDate ) and DepartmentManager . ToDate and count ( FromDate ) GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>natural join staff with address AND THEN natural join address with city AND THEN natural join city with country AND THEN FROM staff as sf WHAT ARE count ( last_update ) and staff . password , username , address . active AND THEN WHAT ARE THE the count of ( last_update ) and address . address IN ( GET staff . store_id , count ( last_name ) IN the staff table AND THEN GROUP AUTOMATICALLY ORDER BY store_id ) as sq_alias where last_update equals foo or address equals bar AND THEN DISPLAY count ( District ) and country . country_id IN table city AND THEN FROM country as cy WHAT ARE staff . last_update , city . Code AND THEN HAVING AVG ( last_update ) equal to 84 LIMIT 8 GROUP AUTOMATICALLY</t>
+          <t>natural join customer with store AND THEN IN customer WHAT IS first_name , count ( customer_id ) AND THEN RETRIEVE store . last_update and store_id IN store AND THEN HAVING AVG ( last_update ) equal to 54 GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>WHAT IS the count of ( FromDate ) , Salaries . FromDate IN Salaries table where ToDate is equal to foo or EmployeeNumber equals bar AND THEN WHAT ARE THE Employees . HireDate and count ( EmployeeNumber ) IN the Employees table AND THEN natural join Salaries with Employees AND THEN GROUP AUTOMATIC HAVING SUM ( HireDate ) equal to 175</t>
+          <t>WHAT ARE THE Title , ToDate IN Titles table where Title is equal to foo or EmployeeNumber is equal to foo HAVING SUM ( Title ) less than 139</t>
         </is>
       </c>
     </row>
@@ -544,7 +544,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FROM the DepartmentManager table PRESENT the count of ( EmployeeNumber ) , DepartmentNumber where FromDate is equal to foo and DepartmentNumber is equal to bar AND THEN PRESENT count ( DepartmentName ) and count ( DepartmentName ) IN departments as ds AND THEN natural join DepartmentManager with departments AND THEN GROUP AUTOMATICALLY</t>
+          <t>IN courseoffering as cg DISPLAY endTime and facultyName HAVING COUNT ( endTime ) equal to 59</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>WHAT ARE THE count ( District ) , last_update , the count of ( Population ) FROM table city as cy AND THEN FIND the sum of ( GNP ) and the average of ( Capital ) FROM ( FROM city table WHAT ARE average ( Population ) , city . Name , city . last_update and the count of ( District ) AND THEN GROUP BY AUTOMATICALLY HAVING SUM ( Name ) greater than 162 ) as sq_alias AND THEN natural join city with country AND THEN GROUP AUTOMATIC</t>
+          <t>WHAT IS term . id , term . endDate FROM term where id is equal to bar and startDate equals bar AND THEN natural join term with term AND THEN natural join term with term AND THEN natural join term with term LIMIT 45 HAVING SUM ( endDate ) greater than 6</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SELECT DepartmentEmployee . DepartmentNumber and the count of ( DepartmentNumber ) , count ( EmployeeNumber ) where FromDate equals foo IN table DepartmentEmployee as De AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>SHOW ME term . startDate and the count of ( termPeriod ) and term . year IN ( RETRIEVE count ( endTime ) and termId FROM table courseoffering HAVING COUNT ( termId ) less than 114 GROUP AUTOMATICALLY ) as sq_aliasGROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -574,7 +574,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>join room with building on room . buildingId equals building . id AND THEN WHAT IS THE building . wheelchairSpaces and the count of ( area ) IN room as rm where id equals bar and area is less than 1661 AND THEN IN building as bg WHAT ARE building . buildingNumber and id AND THEN HAVING AVG ( id ) equal to 124 LIMIT 4 GROUP BY AUTOMATIC</t>
+          <t>RETRIEVE last_update and city IN the city table HAVING AVG ( city ) less than 43</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>natural join city with country AND THEN PRESENT country_id , city_id where Population is less than 1623 and ID IN ( FIND District FROM TABLE country ) FROM city table AND THEN IN the country table as cy FIND sum ( Population ) and Code AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>FROM DepartmentManager as Dr SELECT FromDate and ToDate and the count of ( ToDate ) where FromDate equals foo and ToDate is equal to bar AND THEN DISPLAY count ( DepartmentNumber ) , DepartmentManager . DepartmentNumber IN ( PRESENT the count of ( EmployeeNumber ) , Salaries . Salary where EmployeeNumber equals foo FROM table Salaries as Ss HAVING AVG ( Salary ) less than 38 GROUP AUTOMATIC ) as sq_alias AND THEN natural join DepartmentManager with departments AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WHAT ARE THE the count of ( EmployeeNumber ) and the count of ( FromDate ) IN the DepartmentManager table as Dr AND THEN GROUP BY AUTOMATIC</t>
+          <t>natural join term with term AND THEN FROM term table SHOW ME term . year , term . startDate</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IN table Titles WHAT IS THE EmployeeNumber and Titles . FromDate where Title equals bar or Title is equal to bar</t>
+          <t>IN table film as fm PRESENT count ( description ) and language_id GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>IN table city FIND countrylanguage . CountryCode and city . District AND THEN IN countrylanguage GET countrylanguage . IsOfficial and city . CountryCode AND THEN natural join city with countrylanguage</t>
+          <t>WHAT IS THE the count of ( onDays ) , the count of ( courseId ) , roomId FROM the courseoffering table as cg where id equals bar GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>join room with building on room . buildingId equals building . id AND THEN WHAT IS the count of ( area ) , room . wheelchairSpaces FROM room table AND THEN DISPLAY the count of ( id ) , id and count ( buildingName ) where buildingNumber IN ( SELECT id IN TABLE room ) FROM table building as bg AND THEN GROUP BY AUTOMATIC</t>
+          <t>WHAT ARE film . release_year , film . last_update FROM the film table where film_id is equal to bar or last_update equals bar</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>WHAT ARE THE customer . email and create_date FROM the customer table as cr AND THEN HAVING SUM ( create_date ) greater than 187</t>
+          <t>PRESENT staff . active , the sum of ( active ) IN table staff GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>FROM DepartmentEmployee table FIND count ( EmployeeNumber ) and count ( ToDate ) AND THEN GROUP BY AUTOMATIC</t>
+          <t>IN term table DISPLAY year , term . termPeriod</t>
         </is>
       </c>
     </row>
@@ -654,7 +654,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FROM city table RETRIEVE the sum of ( Population ) and the count of ( last_update ) AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>RETRIEVE country . city_id , country . CountryCode where Name is equal to bar and country_id equals bar FROM city AND THEN WHAT ARE THE average ( GNPOld ) and the average of ( GNP ) and country . Continent FROM country as cy AND THEN natural join city with country AND THEN LIMIT 45 GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -664,7 +664,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>IN DepartmentManager as Dr WHAT IS THE DepartmentManager . FromDate , DepartmentManager . ToDate where FromDate IN ( FIND ToDate IN TABLE DepartmentManager ) and DepartmentNumber is equal to foo AND THEN GROUP AUTOMATIC</t>
+          <t>RETRIEVE manager_staff_id , store . last_update FROM the store table as se where last_update equals bar or address_id equals bar</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>WHAT IS THE sum ( units ) , department . code FROM the course table as ce where units is equal to 1127 or id is equal to foo AND THEN IN table department FIND the count of ( departmentName ) , the count of ( id ) , department . departmentName where departmentName equals foo AND THEN join course with department on course . deptId equals department . id AND THEN GROUP AUTOMATICALLY</t>
+          <t>WHAT IS city . city , average ( Population ) where city_id is equal to bar and city_id is equal to bar IN the city table GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>natural join city with countrylanguage AND THEN IN city as cy where city_id is equal to bar or Population equals 1446 GET Population , CountryCode and average ( Population ) AND THEN FROM table countrylanguage WHAT ARE THE countrylanguage . CountryCode , Percentage and count ( IsOfficial ) and average ( Percentage ) , city . IsOfficial AND THEN GROUP BY AUTOMATIC HAVING COUNT ( CountryCode ) less than 58</t>
+          <t>join courseoffering with room on courseoffering . roomId equals room . id AND THEN join room with building on room . buildingId equals building . id AND THEN PRESENT courseId and facultyName , average ( capacity ) where startTime is equal to foo and id equals bar FROM table courseoffering as cg AND THEN IN room DISPLAY building . buildingId , building . wheelchairSpaces AND THEN IN table building WHAT IS count ( buildingNumber ) and the count of ( id ) and id where buildingName IN ( FIND buildingNumber FROM TABLE building ) AND THEN HAVING SUM ( id ) greater than 65 GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>natural join city with country AND THEN IN table city as cy SELECT ID and city_id AND THEN FROM table country where Name is equal to bar GET the count of ( Code ) and city . GNP AND THEN GROUP AUTOMATICALLY</t>
+          <t>natural join city with countrylanguage AND THEN SELECT CountryCode and the sum of ( Population ) FROM table city as cy where country_id equals bar or ID is equal to bar AND THEN IN ( PRESENT city . District and city . city_id and city . city IN table city ) as sq_alias where IsOfficial is equal to bar or Percentage is equal to 1870 FIND countrylanguage . Language , IsOfficial AND THEN ORDER BY Language DESC GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>natural join city with countrylanguage AND THEN WHAT ARE sum ( Population ) , city . Population , count ( city_id ) IN city AND THEN GET IsOfficial and city . CountryCode FROM the countrylanguage table as ce where Percentage equal to 441 and Language is equal to foo AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>IN table room as rm where roomNumber IN ( FIND buildingId FROM TABLE room ) and floor IN ( FIND area FROM TABLE room ) WHAT ARE id and the sum of ( capacity ) LIMIT 33 GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -714,7 +714,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>IN table city as cy where city is equal to bar and ID IN ( SELECT city_id FROM city ) WHAT ARE THE city . District and sum ( Population ) AND THEN GROUP AUTOMATIC</t>
+          <t>natural join Salaries with Employees AND THEN FROM table Salaries as Ss SELECT Salaries . EmployeeNumber , the count of ( ToDate ) AND THEN RETRIEVE LastName , EmployeeNumber where Gender is equal to foo or LastName is equal to bar FROM table Employees as Es AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FROM Titles as Ts WHAT IS THE the count of ( Title ) and count ( EmployeeNumber ) AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>PRESENT count ( store_id ) and inventory . inventory_id and last_update where store_id equals bar IN the inventory table as iy HAVING AVG ( last_update ) less than 63 GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>join courseoffering with term on courseoffering . termId equals term . id AND THEN natural join term with term AND THEN FROM the courseoffering table WHAT IS endTime , term . roomId AND THEN FROM table term as tm where id is equal to bar WHAT IS THE courseoffering . year , the count of ( termPeriod ) AND THEN GROUP BY AUTOMATIC</t>
+          <t>WHAT ARE THE average ( length ) and the count of ( last_update ) and language . title FROM film table AND THEN IN the language table FIND language_id , name where language_id is equal to foo and name equals bar AND THEN natural join film with language AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SELECT the count of ( EmployeeNumber ) , count ( FromDate ) where DepartmentNumber is equal to foo and EmployeeNumber IN ( DISPLAY ToDate FROM departments ) FROM DepartmentEmployee table AND THEN SELECT count ( DepartmentName ) and DepartmentName FROM table departments AND THEN natural join DepartmentEmployee with departments AND THEN HAVING COUNT ( DepartmentName ) less than 79 GROUP AUTOMATICALLY</t>
+          <t>IN table term as tm where year greater than 1716 WHAT IS THE the sum of ( year ) , term . termPeriod and term . id GROUP BY AUTOMATICALLY LIMIT 43</t>
         </is>
       </c>
     </row>
@@ -754,7 +754,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FROM rental table SELECT inventory_id , address . rental_date and rental . customer_id and the count of ( inventory_id ) AND THEN WHAT IS picture and count ( last_update ) IN staff as sf AND THEN FROM the address table as as where address_id equals bar or address_id equals foo PRESENT staff . location and staff . phone , address_id AND THEN natural join rental with staff AND THEN natural join staff with address AND THEN GROUP AUTOMATIC</t>
+          <t>natural join Salaries with Employees AND THEN IN table Salaries where EmployeeNumber is equal to foo or Salary is less than 1239 WHAT IS THE FromDate and Salary and Salaries . ToDate and EmployeeNumber AND THEN IN Employees table where HireDate is equal to bar WHAT ARE the count of ( FirstName ) and Employees . BirthDate AND THEN GROUP AUTOMATIC LIMIT 12</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PRESENT address . address2 and postal_code IN address as as AND THEN IN city as cy where city_id is equal to foo WHAT ARE address . District , address . city AND THEN natural join address with city AND THEN HAVING SUM ( District ) greater than 62</t>
+          <t>natural join store with address AND THEN natural join address with city AND THEN FROM the store table GET manager_staff_id and city . store_id AND THEN RETRIEVE postal_code and store . district and phone FROM the address table AND THEN IN ( FROM ( WHAT IS THE city_id , count ( address2 ) FROM table address as as GROUP AUTOMATIC HAVING SUM ( city_id ) equal to 75 ) as sq_alias FIND store . manager_staff_id and count ( manager_staff_id ) GROUP BY AUTOMATIC ) as sq_alias where city is equal to foo or Name is equal to bar FIND city . CountryCode and average ( Population ) AND THEN GROUP BY AUTOMATICALLY HAVING COUNT ( CountryCode ) less than 47</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IN city table WHAT IS THE city . city_id and count ( country_id ) and countrylanguage . country_id where city IN ( SELECT ID FROM TABLE city ) AND THEN FROM the countrylanguage table SELECT countrylanguage . IsOfficial and count ( CountryCode ) where Percentage is greater than 1333 or CountryCode IN ( DISPLAY Percentage FROM city ) AND THEN natural join city with countrylanguage AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>FROM customer table RETRIEVE average ( active ) , the count of ( email ) , count ( last_name ) , active where store_id equals bar and customer_id is equal to bar ORDER BY active DESC GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>natural join DepartmentEmployee with departments AND THEN IN the DepartmentEmployee table as De SHOW ME DepartmentEmployee . ToDate , the count of ( EmployeeNumber ) AND THEN IN departments as ds where DepartmentNumber is equal to bar FIND the count of ( DepartmentName ) and DepartmentNumber AND THEN LIMIT 13 HAVING SUM ( DepartmentNumber ) greater than 25 GROUP BY AUTOMATIC</t>
+          <t>FROM Salaries table where FromDate IN ( DISPLAY ToDate IN TABLE Employees ) and Salary equal to 632 WHAT ARE THE the average of ( Salary ) and Salaries . ToDate AND THEN FROM the Employees table RETRIEVE EmployeeNumber and LastName AND THEN natural join Salaries with Employees AND THEN GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>join room with building on room . buildingId equals building . id AND THEN RETRIEVE buildingId and area IN the room table AND THEN WHAT IS the count of ( id ) , the count of ( buildingNumber ) where buildingName IN ( SELECT id IN TABLE room ) FROM table building as bg AND THEN GROUP AUTOMATIC</t>
+          <t>FROM Salaries table SELECT FromDate and sum ( Salary ) GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -804,7 +804,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>natural join city with countrylanguage AND THEN DISPLAY the sum of ( Population ) and ID IN the city table where city is equal to bar or country_id equals foo AND THEN SHOW ME CountryCode and the count of ( IsOfficial ) and countrylanguage . Percentage FROM table countrylanguage where IsOfficial equals foo AND THEN ORDER BY Percentage DESC GROUP BY AUTOMATICALLY</t>
+          <t>natural join Titles with Employees AND THEN PRESENT ToDate and Titles . Title , count ( FromDate ) where ToDate IN ( FIND ToDate IN TABLE Employees ) IN the Titles table AND THEN GET the count of ( HireDate ) and the count of ( HireDate ) IN Employees table AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>natural join DepartmentEmployee with departments AND THEN PRESENT DepartmentNumber , the count of ( ToDate ) where DepartmentNumber is equal to bar FROM the DepartmentEmployee table as De AND THEN WHAT IS DepartmentEmployee . DepartmentNumber , DepartmentEmployee . DepartmentName IN departments as ds AND THEN ORDER BY DepartmentNumber HAVING SUM ( DepartmentNumber ) greater than 150 LIMIT 15 GROUP AUTOMATICALLY</t>
+          <t>DISPLAY sum ( Population ) and city . last_update FROM the city table GROUP BY AUTOMATIC HAVING COUNT ( last_update ) less than 158</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>GET location and the count of ( district ) IN the address table where address is equal to bar and phone is equal to bar AND THEN GROUP BY AUTOMATIC</t>
+          <t>IN Salaries table RETRIEVE Employees . ToDate and the count of ( FromDate ) AND THEN RETRIEVE Gender and Employees . BirthDate , the count of ( EmployeeNumber ) FROM Employees as Es where HireDate is equal to foo AND THEN natural join Salaries with Employees AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>GET sum ( year ) and endDate , the average of ( year ) FROM term table AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>IN city where District equals foo DISPLAY the count of ( ID ) and country . Population AND THEN WHAT IS country . LocalName , city . LifeExpectancy and country . Capital FROM table country as cy where SurfaceArea less than 147 and Region is equal to bar AND THEN natural join city with country AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -844,7 +844,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>WHAT ARE countrylanguage . District and city . Name FROM city AND THEN FROM the countrylanguage table WHAT IS THE average ( Percentage ) and the count of ( Percentage ) and city . Percentage AND THEN natural join city with countrylanguage AND THEN GROUP BY AUTOMATICALLY HAVING SUM ( Percentage ) equal to 161</t>
+          <t>WHAT ARE facultyName and average ( capacity ) IN the courseoffering table AND THEN IN the term table PRESENT the sum of ( year ) and term . termPeriod and sum ( year ) AND THEN join courseoffering with term on courseoffering . termId equals term . id AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DISPLAY language . film_id , the count of ( store_id ) and inventory_id FROM table inventory AND THEN SHOW ME the count of ( film_id ) and language . last_update IN the film table AND THEN FROM language where name equals bar and name equals bar WHAT ARE last_update , language_id AND THEN natural join inventory with film AND THEN natural join film with language AND THEN GROUP AUTOMATIC</t>
+          <t>natural join DepartmentManager with departments AND THEN WHAT IS THE departments . DepartmentNumber , EmployeeNumber where DepartmentNumber is equal to bar FROM table DepartmentManager as Dr AND THEN IN table departments as ds WHAT IS count ( DepartmentName ) and DepartmentManager . DepartmentNumber , DepartmentName AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -864,7 +864,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>IN the rental table as rl WHAT IS rental_id and customer . inventory_id AND THEN WHAT IS active and customer . last_update and store . customer_id , store . last_name and store . first_name IN customer table where first_name is equal to bar AND THEN IN the store table as se where last_update is equal to bar DISPLAY last_update and rental . store_id AND THEN natural join rental with customer AND THEN natural join customer with store</t>
+          <t>IN table rental where customer_id IN ( FIND rental_date FROM rental ) RETRIEVE the count of ( return_date ) , inventory_id AND THEN WHAT IS first_name and address_id IN the staff table AND THEN WHAT IS THE count ( address_id ) and rental . manager_staff_id where store_id equals bar and last_update IN ( FIND address_id FROM rental ) IN table store AND THEN natural join rental with staff AND THEN natural join staff with store AND THEN join store with staff on store . manager_staff_id equals staff . staff_id AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -874,7 +874,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>IN Salaries WHAT ARE the count of ( ToDate ) , Salary , EmployeeNumber AND THEN SELECT FirstName and the count of ( LastName ) IN table Employees where EmployeeNumber is equal to bar or LastName is equal to foo AND THEN natural join Salaries with Employees AND THEN GROUP AUTOMATICALLY</t>
+          <t>FROM city as cy where CountryCode IN ( SELECT city_id IN TABLE city ) DISPLAY city . CountryCode , count ( CountryCode ) , average ( Population ) , District HAVING SUM ( District ) equal to 48 GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -884,7 +884,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SHOW ME city . Name and average ( Population ) FROM the city table as cy AND THEN IN country WHAT IS THE count ( Code ) , GovernmentForm AND THEN natural join city with country AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>FROM table term as tm SHOW ME count ( id ) and termPeriod HAVING AVG ( termPeriod ) equal to 92 GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -894,7 +894,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FIND CountryCode , Population where city IN ( FIND city_id FROM TABLE city ) IN table city AND THEN GROUP AUTOMATIC HAVING AVG ( CountryCode ) greater than 34</t>
+          <t>IN DepartmentManager WHAT IS departments . DepartmentNumber , ToDate AND THEN WHAT ARE DepartmentManager . DepartmentNumber and the count of ( DepartmentName ) and count ( DepartmentName ) FROM departments AND THEN natural join DepartmentManager with departments AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -904,7 +904,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>natural join Titles with Employees AND THEN FROM Titles as Ts SELECT the count of ( Title ) , Titles . FromDate AND THEN FROM table Employees where FirstName equals foo and Gender equals foo GET Employees . HireDate , Titles . Gender AND THEN GROUP BY AUTOMATIC</t>
+          <t>natural join city with country AND THEN PRESENT country . country_id , ID and Population where country_id is equal to bar or city equals foo FROM city as cy AND THEN IN the country table WHAT ARE THE sum ( LifeExpectancy ) and LocalName and Code2 AND THEN HAVING AVG ( LocalName ) equal to 53 GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -914,7 +914,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>IN the rental table as rl PRESENT rental_date , rental . rental_id AND THEN ORDER BY rental_id DESC</t>
+          <t>natural join DepartmentManager with departments AND THEN FROM DepartmentManager as Dr WHAT IS THE ToDate , EmployeeNumber AND THEN FROM table departments as ds where DepartmentNumber is equal to bar and DepartmentNumber is equal to bar WHAT IS THE departments . DepartmentNumber , count ( DepartmentNumber ) AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -924,7 +924,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>join course with department on course . deptId equals department . id AND THEN FROM table course SELECT department . deptId , sum ( units ) and average ( units ) AND THEN IN ( WHAT IS THE termPeriod and the count of ( termPeriod ) and sum ( year ) , startDate FROM term table where year is less than 775 or startDate equals bar AND THEN LIMIT 10 GROUP AUTOMATICALLY ) as sq_alias WHAT ARE THE id , departmentName , _CN_ AND THEN GROUP AUTOMATICALLY</t>
+          <t>SELECT count ( inventory_id ) and film_id IN the inventory table as iy AND THEN WHAT IS THE the count of ( film_id ) and length FROM the film table AND THEN natural join inventory with film AND THEN GROUP BY AUTOMATICALLY LIMIT 42</t>
         </is>
       </c>
     </row>
@@ -934,7 +934,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FROM table store where manager_staff_id equals foo or store_id is equal to bar WHAT IS address_id and store_id</t>
+          <t>IN city table PRESENT sum ( Population ) , city . ID AND THEN SHOW ME city . Language and CountryCode and average ( Percentage ) , the sum of ( Percentage ) IN the countrylanguage table as ce where CountryCode is equal to foo and Language equals foo AND THEN natural join city with countrylanguage AND THEN HAVING COUNT ( Language ) greater than 43 GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>join courseoffering with room on courseoffering . roomId equals room . id AND THEN PRESENT the sum of ( capacity ) and courseoffering . id where roomId equals foo and courseId is equal to bar FROM courseoffering table AND THEN WHAT IS the average of ( area ) and id , courseoffering . area FROM room table AND THEN GROUP AUTOMATICALLY</t>
+          <t>IN table courseoffering FIND term . startTime and term . courseId where roomId is equal to foo and capacity less than 490 AND THEN IN term DISPLAY the sum of ( year ) and term . termPeriod AND THEN join courseoffering with term on courseoffering . termId equals term . id AND THEN natural join term with term AND THEN natural join term with term AND THEN HAVING AVG ( termPeriod ) greater than 177 GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>IN room table where id equals foo WHAT IS THE room . wheelchairSpaces , room . floor and capacity AND THEN LIMIT 14</t>
+          <t>natural join Titles with Employees AND THEN IN table Titles where FromDate IN ( SELECT Title FROM Titles ) GET Title , count ( ToDate ) AND THEN IN the Employees table as Es PRESENT count ( HireDate ) , LastName where Gender is equal to foo AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>WHAT ARE DepartmentEmployee . ToDate , EmployeeNumber IN ( WHAT ARE THE DepartmentNumber , DepartmentManager . EmployeeNumber FROM table DepartmentManager ) as sq_alias AND THEN GROUP AUTOMATICALLY</t>
+          <t>WHAT ARE the sum of ( Salary ) , the count of ( EmployeeNumber ) where Salary equals 1150 and FromDate equals foo IN the Salaries table as SsGROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -974,7 +974,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>IN DepartmentEmployee table RETRIEVE count ( EmployeeNumber ) and count ( EmployeeNumber ) where ToDate equals bar AND THEN GROUP BY AUTOMATIC</t>
+          <t>natural join DepartmentManager with departments AND THEN IN the DepartmentManager table DISPLAY ToDate , departments . FromDate AND THEN RETRIEVE count ( DepartmentNumber ) , DepartmentManager . DepartmentNumber FROM ( WHAT ARE Salaries . EmployeeNumber , Salaries . Salary , the average of ( Salary ) FROM the Salaries table HAVING AVG ( EmployeeNumber ) greater than 31 GROUP BY AUTOMATICALLY ) as sq_alias AND THEN HAVING SUM ( DepartmentNumber ) equal to 67 GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>RETRIEVE endTime , courseoffering . onDays FROM courseoffering table AND THEN SELECT year , the sum of ( year ) , sum ( year ) FROM term as tm where id is equal to foo or termPeriod equals foo AND THEN join courseoffering with term on courseoffering . termId equals term . id AND THEN natural join term with term AND THEN GROUP BY AUTOMATIC</t>
+          <t>WHAT ARE THE DepartmentManager . DepartmentNumber , FromDate where FromDate is equal to bar and ToDate equals foo IN table DepartmentManager HAVING COUNT ( DepartmentNumber ) less than 108</t>
         </is>
       </c>
     </row>
@@ -994,7 +994,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>IN table Salaries as Ss SELECT ToDate and sum ( Salary ) , sum ( Salary ) AND THEN WHAT IS Salaries . Gender , Employees . HireDate , count ( FirstName ) FROM table Employees AND THEN natural join Salaries with Employees AND THEN GROUP AUTOMATICALLY</t>
+          <t>natural join DepartmentManager with departments AND THEN FROM ( FROM table Titles RETRIEVE Titles . Title , ToDate , count ( EmployeeNumber ) GROUP BY AUTOMATIC ) as sq_alias where DepartmentNumber is equal to foo PRESENT count ( FromDate ) , departments . ToDate AND THEN PRESENT departments . DepartmentName , DepartmentNumber IN table departments AND THEN LIMIT 40 GROUP BY AUTOMATIC HAVING AVG ( DepartmentNumber ) equal to 199</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>IN city table RETRIEVE city . city , city . District AND THEN LIMIT 41</t>
+          <t>natural join city with country AND THEN SHOW ME the sum of ( Population ) , country . ID where city_id IN ( DISPLAY city_id FROM TABLE country ) or ID is equal to foo IN city table AND THEN SHOW ME country and city . Region IN the country table as cy where country IN ( DISPLAY last_update FROM TABLE country ) AND THEN GROUP AUTOMATICALLY ORDER BY Region</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>WHAT IS count ( EmployeeNumber ) and DepartmentEmployee . ToDate IN table DepartmentEmployee as De AND THEN HAVING COUNT ( ToDate ) equal to 172 LIMIT 23 ORDER BY ToDate ASC GROUP AUTOMATICALLY</t>
+          <t>WHAT IS city . Name and city . CountryCode , average ( Population ) and city . country_id where ID equals foo IN city GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DISPLAY Employees . ToDate , the count of ( EmployeeNumber ) FROM the Titles table where Title equals foo AND THEN DISPLAY Employees . BirthDate and Employees . LastName where Gender equals foo or Gender IN ( FIND FirstName IN TABLE Titles ) FROM ( FROM the Salaries table WHAT ARE THE ToDate , Salaries . Salary AND THEN LIMIT 32 ORDER BY Salary ASC ) as sq_alias AND THEN natural join Titles with Employees AND THEN GROUP AUTOMATICALLY ORDER BY BirthDate HAVING COUNT ( BirthDate ) greater than 137</t>
+          <t>WHAT ARE THE country . city , the average of ( Population ) , country . ID IN table city as cy AND THEN DISPLAY country . IndepYear , country . GNPOld , city . HeadOfState and country . Capital FROM the country table AND THEN natural join city with country AND THEN GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>RETRIEVE the count of ( city ) and average ( Population ) FROM city as cy AND THEN FROM the country table FIND country . country_id and LocalName , the count of ( last_update ) where SurfaceArea greater than 430 or Continent equals foo AND THEN natural join city with country AND THEN GROUP BY AUTOMATIC</t>
+          <t>RETRIEVE the count of ( ToDate ) , ToDate where FromDate equals bar and EmployeeNumber is equal to bar IN DepartmentManager GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>FROM room table DISPLAY count ( buildingId ) , area , the average of ( capacity ) , average ( capacity ) AND THEN IN the building table as bg where id is equal to bar and buildingName equals bar SELECT building . id and buildingNumber and count ( id ) AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP AUTOMATICALLY</t>
+          <t>FROM table city as cy SHOW ME city . District , the average of ( Population ) GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>natural join DepartmentEmployee with departments AND THEN FROM table DepartmentEmployee as De DISPLAY DepartmentEmployee . ToDate , departments . DepartmentNumber , departments . FromDate , EmployeeNumber and _CN_ where ToDate is equal to foo AND THEN DISPLAY DepartmentName and count ( DepartmentNumber ) , count ( DepartmentNumber ) FROM departments as ds AND THEN GROUP AUTOMATIC</t>
+          <t>natural join city with countrylanguage AND THEN WHAT IS THE the count of ( last_update ) , city_id where city is equal to bar or last_update is equal to bar IN city AND THEN FROM countrylanguage table SHOW ME IsOfficial and average ( Percentage ) and the count of ( Percentage ) , the average of ( Percentage ) where Percentage is equal to 408 or IsOfficial equals bar AND THEN GROUP AUTOMATIC LIMIT 33</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>IN table Salaries where EmployeeNumber equals bar RETRIEVE sum ( Salary ) and the count of ( ToDate ) , Employees . ToDate AND THEN IN ( IN table Salaries as Ss DISPLAY average ( Salary ) , the count of ( FromDate ) , the sum of ( Salary ) AND THEN GROUP BY AUTOMATICALLY ) as sq_alias DISPLAY BirthDate and the count of ( LastName ) where LastName is equal to bar AND THEN natural join Salaries with Employees AND THEN GROUP AUTOMATIC HAVING COUNT ( BirthDate ) equal to 2</t>
+          <t>natural join DepartmentEmployee with departments AND THEN IN DepartmentEmployee table where EmployeeNumber is equal to foo WHAT IS count ( ToDate ) , DepartmentEmployee . DepartmentNumber AND THEN SHOW ME DepartmentName and count ( DepartmentName ) FROM table departments AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>GET city . Population and the count of ( country_id ) , city . ID IN table city as cy where District equals foo or city is equal to foo AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>IN ( IN courseoffering as cg where startTime is equal to bar or onDays is equal to foo WHAT ARE THE startTime and count ( capacity ) GROUP BY AUTOMATICALLY ) as sq_alias GET courseoffering . onDays and roomId , startTime , the average of ( capacity ) AND THEN WHAT IS THE course . deptId , id FROM course as ce AND THEN FROM the department table as dt GET id , course . departmentName AND THEN join courseoffering with course on courseoffering . courseId equals course . id AND THEN join course with department on course . deptId equals department . id AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>natural join film with language AND THEN SHOW ME language . release_year and original_language_id FROM film AND THEN FROM language as le RETRIEVE count ( last_update ) , film . name where name is equal to bar or language_id equals foo AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>natural join city with countrylanguage AND THEN FROM the city table WHAT IS THE the sum of ( Population ) , city , city_id AND THEN RETRIEVE city . IsOfficial , countrylanguage . Percentage and CountryCode FROM the countrylanguage table where IsOfficial is equal to bar AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>natural join rental with staff AND THEN natural join staff with address AND THEN IN rental as rl SELECT customer_id , address . rental_date AND THEN WHAT IS THE email and staff . password FROM table staff where store_id IN ( FIND last_name IN TABLE address ) AND THEN IN address table where city_id IN ( FIND address2 FROM TABLE rental ) and last_update equals bar SHOW ME location and staff . city_id , address . address_id AND THEN GROUP BY AUTOMATIC</t>
+          <t>DISPLAY ToDate , EmployeeNumber IN Titles HAVING SUM ( ToDate ) less than 64</t>
         </is>
       </c>
     </row>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>WHAT IS THE the count of ( rental_id ) and rental_date FROM rental where last_update equals foo or inventory_id IN ( DISPLAY inventory_id FROM TABLE customer ) AND THEN PRESENT rental . active , average ( active ) IN customer table where store_id equals foo or email is equal to bar AND THEN natural join rental with customer AND THEN GROUP BY AUTOMATIC</t>
+          <t>FROM table DepartmentManager as Dr SELECT the count of ( DepartmentNumber ) , the count of ( DepartmentNumber ) and FromDate where DepartmentNumber is equal to foo or ToDate equals foo AND THEN IN the departments table WHAT ARE THE departments . DepartmentNumber and DepartmentManager . DepartmentName AND THEN natural join DepartmentManager with departments AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>FROM the store table where address_id is equal to bar or address_id is equal to foo RETRIEVE address_id and the count of ( store_id ) AND THEN FROM the staff table as sf PRESENT the sum of ( active ) and sum ( active ) where last_update is equal to foo AND THEN IN address GET the count of ( location ) , staff . city_id AND THEN IN table city SHOW ME ID , city . District , store . CountryCode AND THEN join store with staff on store . manager_staff_id equals staff . staff_id AND THEN natural join staff with address AND THEN natural join address with city AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>WHAT IS THE DepartmentManager . FromDate , the count of ( ToDate ) and DepartmentManager . ToDate IN the DepartmentManager table where EmployeeNumber IN ( SELECT DepartmentNumber FROM DepartmentManager ) or DepartmentNumber is equal to bar HAVING SUM ( FromDate ) less than 97 GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>IN the room table where roomNumber is equal to bar or capacity equals 129 SHOW ME room . wheelchairSpaces and building . capacity AND THEN RETRIEVE building . id , count ( id ) FROM the building table AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>IN courseoffering where termId is equal to bar SHOW ME the average of ( capacity ) and count ( termId ) GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>IN city table WHAT IS THE the count of ( Name ) , the average of ( Population ) and city . District AND THEN HAVING SUM ( District ) greater than 154 GROUP AUTOMATIC LIMIT 19</t>
+          <t>natural join DepartmentManager with departments AND THEN FROM DepartmentManager GET DepartmentManager . FromDate , count ( ToDate ) AND THEN IN departments as ds GET DepartmentName and DepartmentNumber where DepartmentName is equal to bar AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>WHAT ARE FromDate , count ( FromDate ) , the count of ( FromDate ) IN Titles as Ts AND THEN LIMIT 9 GROUP AUTOMATICALLY ORDER BY FromDate ASC HAVING SUM ( FromDate ) greater than 51</t>
+          <t>WHAT ARE THE Titles . FromDate , the count of ( EmployeeNumber ) where ToDate equals foo and Title equals foo FROM Titles GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>IN the film table WHAT IS THE the average of ( length ) , film . rating , rental_rate and film . rental_duration and language_id AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>natural join address with city AND THEN natural join city with country AND THEN RETRIEVE city . last_update , postal_code IN ( SHOW ME last_update , payment_date IN table payment where customer_id equals foo ) as sq_alias AND THEN FROM table city FIND country . country_id and count ( country_id ) , city . District , city . Name where city_id is equal to foo or city_id IN ( DISPLAY last_update FROM TABLE city ) AND THEN DISPLAY count ( Code ) , IndepYear and city . GovernmentForm , address . Region IN country table AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>FROM table room as rm where area equals 471 or floor IN ( DISPLAY id FROM building ) GET room . roomNumber and floor AND THEN IN building DISPLAY the count of ( buildingName ) and count ( buildingNumber ) and room . id AND THEN join room with building on room . buildingId equals building . id AND THEN LIMIT 14 GROUP BY AUTOMATIC</t>
+          <t>FROM city table WHAT ARE THE Name and city . Population where Population greater than 1874 or last_update is equal to bar HAVING AVG ( Population ) greater than 133</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>natural join city with country AND THEN RETRIEVE country . country_id and count ( District ) IN ( SHOW ME city . CountryCode , city FROM city as cy ) as sq_alias AND THEN IN the country table SHOW ME count ( Region ) , last_update and average ( LifeExpectancy ) AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>FROM film where release_year equals foo WHAT ARE the count of ( length ) and title , rating GROUP BY AUTOMATICALLY HAVING SUM ( rating ) greater than 65</t>
         </is>
       </c>
     </row>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>SELECT store . address_id and last_update where address_id IN ( SELECT address_id IN TABLE store ) or manager_staff_id equals bar IN the store table AND THEN LIMIT 31 ORDER BY last_update ASC GROUP AUTOMATIC</t>
+          <t>IN the city table as cy PRESENT country . ID and sum ( Population ) , sum ( Population ) AND THEN IN country table WHAT ARE THE average ( SurfaceArea ) , sum ( Capital ) and country . LocalName AND THEN natural join city with country AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>IN ( WHAT ARE EmployeeNumber and the count of ( Title ) , FromDate , ToDate FROM Titles table where FromDate equals foo and EmployeeNumber is equal to bar AND THEN GROUP AUTOMATIC ) as sq_alias where EmployeeNumber equals bar or Salary is less than 1779 FIND FromDate , Salaries . Salary , EmployeeNumber and average ( Salary ) AND THEN HAVING COUNT ( FromDate ) equal to 82 GROUP BY AUTOMATIC LIMIT 42</t>
+          <t>DISPLAY courseoffering . id , capacity , sum ( capacity ) , sum ( capacity ) IN courseoffering as cg GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>PRESENT Salaries . ToDate , Salaries . EmployeeNumber , Employees . Salary FROM ( WHAT ARE the count of ( FromDate ) and EmployeeNumber IN the Titles table where EmployeeNumber is equal to foo or EmployeeNumber IN ( DISPLAY FromDate FROM TABLE Titles ) AND THEN GROUP BY AUTOMATIC ) as sq_alias AND THEN IN the Employees table as Es SHOW ME LastName and HireDate AND THEN natural join Salaries with Employees AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>PRESENT customer_id , rental_id , rental . return_date FROM rental as rl HAVING SUM ( return_date ) less than 85</t>
         </is>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>WHAT ARE THE city . last_update , sum ( Population ) IN table city AND THEN SHOW ME city . HeadOfState and the count of ( last_update ) IN table country as cy where LocalName is equal to foo or Code equals foo AND THEN natural join city with country AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>natural join Titles with Employees AND THEN FIND count ( FromDate ) and Titles . Title where ToDate equals bar or EmployeeNumber IN ( FIND ToDate FROM Employees ) IN ( IN the DepartmentManager table as Dr where DepartmentNumber is equal to bar WHAT ARE the count of ( EmployeeNumber ) and the count of ( ToDate ) GROUP BY AUTOMATICALLY ) as sq_alias AND THEN IN the Employees table RETRIEVE FirstName , Employees . HireDate AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>FROM film table FIND language . length , language . replacement_cost where title is equal to foo or last_update is equal to foo AND THEN SELECT last_update , language . language_id and film . name IN language table AND THEN natural join film with language</t>
+          <t>IN table Salaries FIND the sum of ( Salary ) , Salary where ToDate equals bar or ToDate IN ( FIND FromDate FROM Employees ) AND THEN FROM the Employees table as Es PRESENT Salaries . FirstName and Employees . HireDate AND THEN natural join Salaries with Employees AND THEN GROUP BY AUTOMATIC ORDER BY FirstName ASC</t>
         </is>
       </c>
     </row>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>natural join staff with store AND THEN join store with staff on store . manager_staff_id equals staff . staff_id AND THEN natural join staff with store AND THEN RETRIEVE staff_id , the average of ( active ) FROM table staff as sf where password equals bar AND THEN IN store as se SHOW ME count ( address_id ) and last_update and store_id AND THEN GROUP AUTOMATIC</t>
+          <t>FROM ( FROM store where manager_staff_id equals bar SELECT the count of ( manager_staff_id ) , address_id and last_updateGROUP AUTOMATIC HAVING COUNT ( last_update ) equal to 35 ) as sq_alias where manager_staff_id equals bar or address_id equals foo WHAT IS THE count ( manager_staff_id ) , the count of ( store_id ) , last_update GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>RETRIEVE last_update and inventory . inventory_id IN inventory where store_id equals bar and inventory_id equals foo</t>
+          <t>WHAT ARE THE wheelchairSpaces and buildingId where id equals bar and capacity equals 1930 IN room HAVING COUNT ( wheelchairSpaces ) equal to 6 LIMIT 17</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>FROM the courseoffering table GET capacity and courseId</t>
+          <t>natural join city with countrylanguage AND THEN PRESENT count ( city ) , city . Population and average ( Population ) FROM table city where District is equal to foo AND THEN WHAT IS THE IsOfficial , CountryCode and the average of ( Percentage ) IN the countrylanguage table as ce where IsOfficial equals foo and Percentage less than 619 AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>FROM DepartmentManager WHAT ARE THE DepartmentNumber and ToDate , count ( EmployeeNumber ) , FromDate AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>IN city as cy where Population less than 1751 and Population equals 1263 GET country_id and the count of ( Population ) GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>FROM city RETRIEVE country_id and city_id and sum ( Population ) , CountryCode , count ( last_update ) AND THEN GROUP BY AUTOMATIC</t>
+          <t>FROM table city as cy PRESENT countrylanguage . last_update and countrylanguage . District and sum ( Population ) AND THEN PRESENT Language and sum ( Percentage ) IN countrylanguage AND THEN natural join city with countrylanguage AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>WHAT ARE THE country_id and city FROM city table where ID is equal to bar and country_id equals foo AND THEN LIMIT 37</t>
+          <t>WHAT ARE count ( Title ) , ToDate FROM table Titles as TsGROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>WHAT ARE city , the sum of ( Population ) and sum ( Population ) and city . city_id IN table city as cy AND THEN GROUP BY AUTOMATIC HAVING COUNT ( city ) equal to 186</t>
+          <t>FROM city table WHAT IS Population and city . Name , last_update where ID IN ( SELECT city_id IN TABLE city ) or District equals foo LIMIT 17 GROUP AUTOMATIC HAVING AVG ( last_update ) equal to 136</t>
         </is>
       </c>
     </row>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>IN city table WHAT ARE city . Name and sum ( Population ) AND THEN ORDER BY Name ASC GROUP AUTOMATICALLY</t>
+          <t>FROM DepartmentManager table WHAT IS THE FromDate , DepartmentManager . ToDate and DepartmentManager . EmployeeNumber and count ( DepartmentNumber ) AND THEN PRESENT count ( DepartmentName ) , DepartmentNumber FROM the departments table AND THEN natural join DepartmentManager with departments AND THEN GROUP AUTOMATICALLY HAVING COUNT ( DepartmentNumber ) equal to 180</t>
         </is>
       </c>
     </row>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>IN the course table as ce RETRIEVE title , code and department . units AND THEN PRESENT course . id , course . departmentName IN department AND THEN join course with department on course . deptId equals department . id AND THEN HAVING AVG ( departmentName ) equal to 93</t>
+          <t>natural join city with country AND THEN FROM table city as cy WHAT ARE count ( CountryCode ) and country_id and country . last_update where Name equals foo and Name is equal to foo AND THEN FROM country table WHAT ARE sum ( Population ) and country . Population where LocalName equals foo and Code2 is equal to bar AND THEN GROUP AUTOMATIC HAVING AVG ( Population ) greater than 117</t>
         </is>
       </c>
     </row>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>natural join city with country AND THEN FIND the average of ( Population ) and the count of ( last_update ) FROM city as cy AND THEN IN country GET city . last_update and city . Population AND THEN GROUP BY AUTOMATIC HAVING AVG ( last_update ) less than 50</t>
+          <t>natural join Salaries with Employees AND THEN FROM Salaries WHAT IS Salaries . Salary , FromDate AND THEN PRESENT Employees . FirstName and EmployeeNumber FROM ( WHAT ARE DepartmentManager . DepartmentNumber , ToDate FROM table DepartmentManager where ToDate IN ( SELECT EmployeeNumber FROM TABLE DepartmentManager ) and ToDate IN ( DISPLAY EmployeeNumber FROM DepartmentManager )GROUP AUTOMATIC LIMIT 23 HAVING AVG ( ToDate ) equal to 58 ) as sq_alias where EmployeeNumber equals foo and EmployeeNumber equals bar AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>IN city table where country_id is equal to bar or District IN ( SELECT last_update FROM city ) WHAT ARE THE city . city_id and city . city AND THEN IN country table where LifeExpectancy is equal to 2033 WHAT ARE THE Region , LocalName AND THEN natural join city with country AND THEN GROUP AUTOMATICALLY</t>
+          <t>SHOW ME staff . store_id and staff . username and staff . email and staff . last_update where username IN ( FIND last_update IN TABLE staff ) and address_id is equal to bar IN staff as sf LIMIT 48 HAVING AVG ( username ) greater than 2 GROUP AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>FROM table store as se DISPLAY manager_staff_id , store_id , the count of ( last_update ) AND THEN WHAT ARE THE address . city_id , address where last_update equals bar IN address as as AND THEN natural join store with address AND THEN GROUP AUTOMATIC</t>
+          <t>WHAT IS courseoffering . id , courseId and average ( capacity ) FROM courseoffering as cg GROUP BY AUTOMATIC HAVING SUM ( id ) greater than 199</t>
         </is>
       </c>
     </row>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>join store with staff on store . manager_staff_id equals staff . staff_id AND THEN natural join staff with address AND THEN natural join address with city AND THEN WHAT IS address_id , manager_staff_id and count ( store_id ) where manager_staff_id equals foo or store_id is equal to foo IN the store table AND THEN WHAT IS THE the sum of ( active ) and count ( username ) , the count of ( last_name ) where store_id is equal to bar and password is equal to foo FROM staff AND THEN FROM table address as as WHAT ARE the count of ( postal_code ) and staff . address_id where address_id is equal to bar and city_id is equal to bar AND THEN WHAT IS address . District , ID FROM table city as cy AND THEN GROUP BY AUTOMATICALLY LIMIT 4</t>
+          <t>RETRIEVE Salary , EmployeeNumber , sum ( Salary ) IN table Salaries GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>FROM table city as cy where Name IN ( SELECT city_id FROM countrylanguage ) SELECT District , count ( Name ) and sum ( Population ) AND THEN FROM table countrylanguage WHAT ARE THE countrylanguage . Percentage and city . IsOfficial where Language is equal to foo or Language equals foo AND THEN natural join city with countrylanguage AND THEN GROUP BY AUTOMATIC LIMIT 11</t>
+          <t>SHOW ME the count of ( EmployeeNumber ) , Employees . Title where Title is equal to foo and EmployeeNumber IN ( SELECT Title FROM TABLE Titles ) FROM Titles as Ts AND THEN GET count ( Gender ) , Employees . Gender , count ( HireDate ) IN Employees AND THEN natural join Titles with Employees AND THEN GROUP BY AUTOMATIC ORDER BY Gender ASC</t>
         </is>
       </c>
     </row>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>FROM the room table WHAT ARE THE room . area and room . capacity</t>
+          <t>IN the city table as cy RETRIEVE the average of ( Population ) , the average of ( Population ) where last_update equals foo and last_update IN ( FIND country_id IN TABLE city ) AND THEN GET countrylanguage . IsOfficial and average ( Percentage ) FROM countrylanguage as ce AND THEN natural join city with countrylanguage AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>natural join DepartmentEmployee with departments AND THEN FROM table DepartmentEmployee as De WHAT IS departments . FromDate , ToDate AND THEN IN the departments table SELECT DepartmentNumber and DepartmentName</t>
+          <t>join course with department on course . deptId equals department . id AND THEN WHAT IS course . id and count ( units ) and units IN table course AND THEN WHAT IS department . id and the count of ( departmentName ) where departmentName is equal to bar FROM the department table AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>FROM Titles table DISPLAY count ( FromDate ) , Titles . Title AND THEN GROUP BY AUTOMATICALLY ORDER BY Title ASC</t>
+          <t>FROM courseoffering as cg where id equals foo WHAT ARE THE endTime and the average of ( capacity ) LIMIT 10 GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>natural join Salaries with Employees AND THEN FROM the Salaries table WHAT IS THE count ( EmployeeNumber ) , FromDate AND THEN RETRIEVE the count of ( LastName ) and Employees . HireDate and FirstName and Salaries . BirthDate , LastName , Employees . EmployeeNumber where Gender IN ( SELECT Gender IN TABLE Employees ) FROM table Employees as Es AND THEN GROUP BY AUTOMATICALLY LIMIT 8</t>
+          <t>WHAT ARE THE sum ( capacity ) , the average of ( capacity ) and the count of ( facultyName ) and term . endTime where termId equals foo FROM the courseoffering table as cg AND THEN IN term table DISPLAY termPeriod , id and term . year , endDate where endDate is equal to foo AND THEN join courseoffering with term on courseoffering . termId equals term . id AND THEN natural join term with term AND THEN natural join term with term AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>SHOW ME the sum of ( units ) , department . units IN course as ce where code is equal to bar AND THEN IN the department table as dt WHAT ARE THE course . departmentName and id , _TN_ . _TNCN_ , the count of ( id ) AND THEN join course with department on course . deptId equals department . id AND THEN GROUP AUTOMATICALLY HAVING AVG ( id ) less than 146</t>
+          <t>natural join DepartmentManager with departments AND THEN FROM DepartmentManager table where DepartmentNumber IN ( SELECT EmployeeNumber FROM TABLE departments ) and DepartmentNumber equals bar WHAT ARE THE DepartmentNumber , count ( DepartmentNumber ) AND THEN FROM departments table SHOW ME DepartmentManager . DepartmentName , departments . DepartmentNumber where DepartmentNumber equals foo AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>join courseoffering with room on courseoffering . roomId equals room . id AND THEN join room with building on room . buildingId equals building . id AND THEN FROM the courseoffering table as cg where id is equal to bar DISPLAY room . onDays and capacity , courseId AND THEN IN room table WHAT IS count ( id ) and the count of ( id ) where roomNumber equals bar and wheelchairSpaces is greater than 816 AND THEN SELECT id and room . buildingName IN building as bg where buildingName is equal to foo or buildingName equals foo AND THEN GROUP AUTOMATICALLY</t>
+          <t>natural join rental with staff AND THEN natural join staff with store AND THEN join store with staff on store . manager_staff_id equals staff . staff_id AND THEN PRESENT customer_id and count ( rental_id ) where inventory_id IN ( FIND return_date FROM TABLE rental ) or return_date is equal to foo IN table rental as rl AND THEN FROM the staff table as sf where username equals bar and last_name IN ( FIND address_id IN TABLE store ) WHAT ARE THE the average of ( active ) , last_name AND THEN RETRIEVE last_update , count ( address_id ) where address_id is equal to foo or last_update IN ( SELECT last_update FROM TABLE staff ) IN table store AND THEN GROUP AUTOMATIC HAVING COUNT ( last_update ) equal to 149</t>
         </is>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>FIND the count of ( roomId ) and capacity and sum ( capacity ) IN courseoffering as cg where id is equal to foo and facultyName is equal to foo AND THEN WHAT IS term . endDate , termPeriod IN term table where termPeriod is equal to bar and startDate is equal to bar AND THEN join courseoffering with term on courseoffering . termId equals term . id AND THEN GROUP AUTOMATICALLY</t>
+          <t>FROM city as cy FIND count ( country_id ) and count ( city ) GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
     </row>

</xml_diff>